<commit_message>
Added code in All Tab, Datatable and AllTab Test classes for Custom Range Date filter on the Page.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Login_Data.xlsx
+++ b/src/test/resources/testdata/Login_Data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7594EC4-F6A4-4EBC-90AF-8CB89D116B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -171,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,11 +484,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F13" sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,21 +742,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4"/>
-    <hyperlink ref="C5" r:id="rId5"/>
-    <hyperlink ref="D5" r:id="rId6"/>
-    <hyperlink ref="C6" r:id="rId7"/>
-    <hyperlink ref="D6" r:id="rId8"/>
-    <hyperlink ref="C7" r:id="rId9"/>
-    <hyperlink ref="D7" r:id="rId10"/>
-    <hyperlink ref="C9" r:id="rId11"/>
-    <hyperlink ref="D10" r:id="rId12"/>
-    <hyperlink ref="D11" r:id="rId13"/>
-    <hyperlink ref="C13" r:id="rId14"/>
-    <hyperlink ref="D12" r:id="rId15"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C13" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D12" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>

</xml_diff>